<commit_message>
day 4 file upatedated
</commit_message>
<xml_diff>
--- a/Day 4 functions.xlsx
+++ b/Day 4 functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL_4\Desktop\Excel 8 to 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7154EE9-2436-41A4-9892-E5D3347C0F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F50AEC-9CE3-4400-82D0-9DED130C9A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C8A77DE6-9EA5-4AE6-BB54-8DE8BCD792C4}"/>
   </bookViews>
@@ -1282,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A055BEC-203F-412B-893C-1D8300377C94}">
   <dimension ref="A2:W89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,7 +1383,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7">
         <f ca="1">RANDBETWEEN(1, 10)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I3" s="7">
         <f>SIGN(E3)</f>
@@ -1460,7 +1460,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7">
         <f t="shared" ref="H4:H16" ca="1" si="0">RANDBETWEEN(1, 10)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" ref="I4:I16" si="1">SIGN(E4)</f>
@@ -1537,7 +1537,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
@@ -1614,7 +1614,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" si="1"/>
@@ -1691,7 +1691,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="1"/>
@@ -1768,7 +1768,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="1"/>
@@ -1845,7 +1845,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
@@ -1922,7 +1922,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="1"/>
@@ -1999,7 +1999,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="1"/>
@@ -2076,7 +2076,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" si="1"/>
@@ -2153,7 +2153,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="1"/>
@@ -2230,7 +2230,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I14" s="7">
         <f t="shared" si="1"/>
@@ -2307,7 +2307,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I15" s="7">
         <f t="shared" si="1"/>
@@ -2384,7 +2384,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I16" s="7">
         <f t="shared" si="1"/>
@@ -4039,6 +4039,10 @@
       <c r="D76" s="2">
         <v>52000</v>
       </c>
+      <c r="E76">
+        <f>FIND("sha", LOWER(A76))</f>
+        <v>9</v>
+      </c>
       <c r="F76" t="str">
         <f>LEFT(A76, 3)</f>
         <v xml:space="preserve">  A</v>

</xml_diff>